<commit_message>
script plz be gentle
</commit_message>
<xml_diff>
--- a/LR3/table_1_10.xlsx
+++ b/LR3/table_1_10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>№ квартиры</t>
   </si>
@@ -143,12 +143,6 @@
     <t>Куропаткин 17</t>
   </si>
   <si>
-    <t>Дата оплаты, дней</t>
-  </si>
-  <si>
-    <t>Срок оплаты, дней</t>
-  </si>
-  <si>
     <t>Максимальный срок просрочки, дней</t>
   </si>
   <si>
@@ -176,7 +170,16 @@
     <t>Средняя площадь, кв.м.</t>
   </si>
   <si>
-    <t>Максимальная сумма к оплате, руб.</t>
+    <t>Срок оплаты</t>
+  </si>
+  <si>
+    <t>Дата оплаты</t>
+  </si>
+  <si>
+    <t>Максимальная сумма, руб.</t>
+  </si>
+  <si>
+    <t>Общая сумма, руб.</t>
   </si>
 </sst>
 </file>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -588,31 +591,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2233,7 +2236,7 @@
     <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C40" s="7">
         <f>FLOOR(SUM(K3:K38), 1)</f>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="41" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="7">
         <f>AVERAGE(C3:C38)</f>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C42" s="7">
         <f>MAX(H3:H38)</f>

</xml_diff>